<commit_message>
Updated image and table
</commit_message>
<xml_diff>
--- a/tables/folders.xlsx
+++ b/tables/folders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\docs\CDM-manual\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-science\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B7AFFBD-2F02-42F1-A091-D358157789E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C53C6B3-B268-4E17-908D-BBC2CA4F750B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8030" yWindow="3200" windowWidth="28800" windowHeight="15650" xr2:uid="{CB6DA50E-5090-4255-AEF7-C8383B51C54F}"/>
+    <workbookView xWindow="6390" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{CB6DA50E-5090-4255-AEF7-C8383B51C54F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Table</t>
   </si>
@@ -44,40 +44,37 @@
     <t>Description</t>
   </si>
   <si>
-    <t>docs</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
-    <t>gis</t>
-  </si>
-  <si>
-    <t>models</t>
-  </si>
-  <si>
-    <t>scripts</t>
-  </si>
-  <si>
-    <t>sandbox</t>
-  </si>
-  <si>
-    <t>Documentation relevent to the CDM repository (including this manual)</t>
-  </si>
-  <si>
-    <t>All raw &amp; processed data, as well as summary images and tables</t>
-  </si>
-  <si>
-    <t>All QGIS project files, GIS data files and summary maps and images</t>
-  </si>
-  <si>
-    <t>All models created and utilised during the project</t>
-  </si>
-  <si>
-    <t>All Matlab, R &amp; Python scripts used to import &amp; process data, as well as model creation</t>
-  </si>
-  <si>
-    <t>All free directory users can add scratch files and temporary datasets</t>
+    <t>data-lake</t>
+  </si>
+  <si>
+    <t>data-governance</t>
+  </si>
+  <si>
+    <t>data-mapping</t>
+  </si>
+  <si>
+    <t>data-warehouse</t>
+  </si>
+  <si>
+    <t>Document repository for data governance</t>
+  </si>
+  <si>
+    <t>Storage of raw, unstructured data</t>
+  </si>
+  <si>
+    <t>GIS mapping information pertaining to the files stored in the data-lake directory</t>
+  </si>
+  <si>
+    <t>Storage for curated datasets.</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Storage for importation pipeline code as well as secondary data products</t>
   </si>
 </sst>
 </file>
@@ -429,15 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FCD7C1-B48B-4E84-8488-073D659691F6}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -454,68 +451,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>